<commit_message>
Data Drive Script is added
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B103_Selenium\workspace2\b103afw\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\git\b103afw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95450FC7-720F-4BD4-8700-9A6160BB7071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47DFF5B-CB95-48FC-9D71-1EE0DC4DC36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +26,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
   <si>
     <t>bhanu</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pointofsale</t>
   </si>
 </sst>
 </file>
@@ -350,7 +360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -369,4 +379,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE312FB9-227E-477B-840D-EC3FC65FFEB0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Made changes added new scripts
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -5,16 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\workspace2_gitExample\b103afw\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\b103afw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCA93B3-AF99-4542-9712-3FC960A5B404}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2F4F79-89BA-48F3-844E-F7F69C4DAE62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
     <sheet name="ValidLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="InVaild_Input1" sheetId="3" r:id="rId3"/>
+    <sheet name="InVaild_Input2" sheetId="4" r:id="rId4"/>
+    <sheet name="InVaild_Input3" sheetId="5" r:id="rId5"/>
+    <sheet name="InVaild_Input4" sheetId="6" r:id="rId6"/>
+    <sheet name="InVaild_Input5" sheetId="7" r:id="rId7"/>
+    <sheet name="InVaild_Input6" sheetId="8" r:id="rId8"/>
+    <sheet name="InVaild_Input7" sheetId="9" r:id="rId9"/>
+    <sheet name="InVaild_Input8" sheetId="10" r:id="rId10"/>
+    <sheet name="InVaild_Input9" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -47,6 +56,24 @@
   </si>
   <si>
     <t>edc</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>sale</t>
+  </si>
+  <si>
+    <t>POINTOFSALE</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>nopoint</t>
   </si>
 </sst>
 </file>
@@ -387,12 +414,74 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B78B46-3A77-452A-8EAB-81CE49818CF3}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C57C4C-EE19-44BA-8E84-69CE8A63F0BD}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE312FB9-227E-477B-840D-EC3FC65FFEB0}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -424,4 +513,221 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BD7417-21AC-46E9-B276-1E5FBBCF64C4}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97EA984-2CD7-4537-BB25-7DBA065C8405}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF69A2B-1047-47E1-A13F-2E30F1CB6A0A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB38A82-15B5-4A82-981C-3EA37AFACAE4}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7A023D-47A2-4C31-8EE0-273EDD6D0DA1}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5D0AF1-CA83-43BF-9B56-0A0DE822117C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5089BD61-D11A-4945-ADD6-B81CC3D8290C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>